<commit_message>
Cambios Calcular Fecha Fin Automatico Subir Cantidad De Dias Adquiridos Automatico Manejar Opcion Para Realizar Consumo Antes Del Termino Del Periodo
</commit_message>
<xml_diff>
--- a/SistVacacionesWeb.UILayer/Plantillas/Plantilla Vacaciones.xlsx
+++ b/SistVacacionesWeb.UILayer/Plantillas/Plantilla Vacaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\source\repos\VS 2019\Web\.NET Framework\SistVacacionesWeb\SistVacacionesWeb.UILayer\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3573F7-7F30-4694-838D-F500753DA21C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D131783-726F-4055-B9A2-47E709E28D5C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{6B37301F-946E-4AA9-AA80-5683ACAE9AAD}"/>
   </bookViews>
@@ -67,6 +67,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>marco</author>
+    <author>Usuario</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{917CCAE8-E3B4-4B0D-8F4B-7A1C5970EFDB}">
@@ -84,7 +85,37 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{088171FE-B8C5-4DE8-A144-47684D3A1E71}">
+    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{65F3E5E8-A93F-42CA-B8B5-A280F5B0D935}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Si: 1
+No: 0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{D43B4E9F-8D14-4D31-9023-90D0ABE77443}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Si: 1
+No: 0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{088171FE-B8C5-4DE8-A144-47684D3A1E71}">
       <text>
         <r>
           <rPr>
@@ -105,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Nombre y Apellidos</t>
   </si>
@@ -141,13 +172,19 @@
   </si>
   <si>
     <t>Código Personal - Anterior</t>
+  </si>
+  <si>
+    <t>¿Usar consumo vacacional antes de terminar el periodo?</t>
+  </si>
+  <si>
+    <t>¿Aplicar Dias Adquiridos Automatico?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +198,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -210,13 +254,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,7 +624,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4A8EE0-92EE-4093-88B7-86CF5F820A66}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -586,12 +633,14 @@
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -601,16 +650,22 @@
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>